<commit_message>
Added correct files after cleanup
</commit_message>
<xml_diff>
--- a/flight_risk_employees.xlsx
+++ b/flight_risk_employees.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>john.arnold@enron.com</t>
+          <t>patti.thompson@enron.com</t>
         </is>
       </c>
     </row>
@@ -464,20 +464,6 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>johnny.palmer@enron.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>patti.thompson@enron.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
           <t>bobette.riner@ipgdirect.com</t>
         </is>
       </c>

</xml_diff>